<commit_message>
Fixed Spelling mistake, improved print function
</commit_message>
<xml_diff>
--- a/SimpleTest_Factors.xlsx
+++ b/SimpleTest_Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\Git\Scenario-Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\Scenario-Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772DBDDD-BAB4-4311-BEA2-78AC6ECFDAC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3E83BA-B5BB-4A01-9192-8AC0B2CD9AE2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="3240" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Bleibt gleich</t>
   </si>
   <si>
-    <t>Fäll</t>
-  </si>
-  <si>
     <t>konstant</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>sehr viel heißer</t>
+  </si>
+  <si>
+    <t>fällt</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +457,7 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -465,10 +465,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -476,10 +476,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>